<commit_message>
feat(java): :sparkles: boolean values handled as test data in excel sheet
Boolean values were not handled correctly as test data. This has been fixed in this ticket
</commit_message>
<xml_diff>
--- a/core-java/src/test/resources/data/excel/BookingData.xlsx
+++ b/core-java/src/test/resources/data/excel/BookingData.xlsx
@@ -1,17 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28207"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED7883B1-AD25-4155-80AD-B0AA397AF7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Bookings" sheetId="1" r:id="rId4"/>
+    <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>SrNo</t>
   </si>
@@ -37,6 +57,9 @@
     <t>AdditionalNeeds</t>
   </si>
   <si>
+    <t>Enabled</t>
+  </si>
+  <si>
     <t>Wasiq</t>
   </si>
   <si>
@@ -68,30 +91,78 @@
   </si>
   <si>
     <t>Breakfast</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Gunner</t>
+  </si>
+  <si>
+    <t>2023-12-11</t>
+  </si>
+  <si>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>Dorothy</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
+  </si>
+  <si>
+    <t>2023-12-09</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Bell</t>
+  </si>
+  <si>
+    <t>2023-12-12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -101,46 +172,49 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -330,23 +404,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="8" max="8" width="14.13"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -371,65 +450,190 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="12.75">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="I2" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="4">
+    <row r="3" spans="1:9" ht="12.75">
+      <c r="A3" s="2">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="12.75">
+      <c r="A4" s="2">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>3000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A5" s="2">
+        <f>A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>6700</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A6" s="2">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>907</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2000.0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
+      <c r="I6" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A7" s="2">
+        <f>A6+1</f>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>987</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="5" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(java): :sparkles: boolean values handled as test data in excel s… (#912)
</commit_message>
<xml_diff>
--- a/core-java/src/test/resources/data/excel/BookingData.xlsx
+++ b/core-java/src/test/resources/data/excel/BookingData.xlsx
@@ -1,17 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28207"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED7883B1-AD25-4155-80AD-B0AA397AF7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Bookings" sheetId="1" r:id="rId4"/>
+    <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>SrNo</t>
   </si>
@@ -37,6 +57,9 @@
     <t>AdditionalNeeds</t>
   </si>
   <si>
+    <t>Enabled</t>
+  </si>
+  <si>
     <t>Wasiq</t>
   </si>
   <si>
@@ -68,30 +91,78 @@
   </si>
   <si>
     <t>Breakfast</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Gunner</t>
+  </si>
+  <si>
+    <t>2023-12-11</t>
+  </si>
+  <si>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>Dorothy</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
+  </si>
+  <si>
+    <t>2023-12-09</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Bell</t>
+  </si>
+  <si>
+    <t>2023-12-12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -101,46 +172,49 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -330,23 +404,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="8" max="8" width="14.13"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -371,65 +450,190 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="12.75">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="I2" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="4">
+    <row r="3" spans="1:9" ht="12.75">
+      <c r="A3" s="2">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="12.75">
+      <c r="A4" s="2">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>3000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A5" s="2">
+        <f>A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>6700</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A6" s="2">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>907</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2000.0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
+      <c r="I6" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A7" s="2">
+        <f>A6+1</f>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>987</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="5" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>